<commit_message>
upload edited .gitignore and other latest files
</commit_message>
<xml_diff>
--- a/Risk Assessment.xlsx
+++ b/Risk Assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashsi\Documents\QA\QA_Project\Inventory Management System - PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashsi\Documents\QA\QA_Project\InventoryManagementSystem-PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C62691-D331-4586-A681-8DE485990242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF197BE-3C64-4690-9E12-500D77EE4BE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{8CB24F64-C717-488D-A877-05C866C4B332}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CB24F64-C717-488D-A877-05C866C4B332}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Project Name:</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Git </t>
+  </si>
+  <si>
+    <t>25.04.2020</t>
   </si>
 </sst>
 </file>
@@ -429,11 +435,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -814,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672790C0-2960-4938-80FA-B969A373BC5B}">
   <dimension ref="A2:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -825,402 +828,406 @@
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" customWidth="1"/>
     <col min="11" max="11" width="30.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="30.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="1"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="1"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="1"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
     </row>
     <row r="7" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="8" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <v>1</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <f>A8+1</f>
         <v>2</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="5" t="s">
+      <c r="G9" s="4"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+    <row r="10" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <f t="shared" ref="A10:A18" si="0">A9+1</f>
         <v>3</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="5" t="s">
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+    <row r="11" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="6" t="s">
+      <c r="G11" s="4"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="2" t="s">
+      <c r="J11" s="4"/>
+      <c r="K11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="6" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="2" t="s">
+      <c r="J13" s="4"/>
+      <c r="K13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+    <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="3" t="s">
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="2" t="s">
+      <c r="I14" s="5"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="B15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="A17" s="11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="11">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="H7:J7"/>
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="D4:L4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
uploading files requested from the checklist
</commit_message>
<xml_diff>
--- a/Risk Assessment.xlsx
+++ b/Risk Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashsi\Documents\QA\QA_Project\InventoryManagementSystem-PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF197BE-3C64-4690-9E12-500D77EE4BE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C5434B-3251-4FA2-8808-4410F1A89E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CB24F64-C717-488D-A877-05C866C4B332}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t>Project Name:</t>
   </si>
@@ -96,72 +96,19 @@
   </si>
   <si>
     <t>Risk area</t>
-  </si>
-  <si>
-    <t>Poor planning. 
-Can start off on track but then fall behind.</t>
-  </si>
-  <si>
-    <t>Not reading the requirements properly.</t>
-  </si>
-  <si>
-    <t>Insufficient practice on programming language.
-Mediocre knowledge of technologies to be used.</t>
   </si>
   <si>
     <t>Errors in entity relationship diagram (ERD).
 Relationships between entities incorrectly defined.</t>
   </si>
   <si>
-    <t>Not meeting deadlines, causing backlog and eventually delay in completion.</t>
-  </si>
-  <si>
     <t>Objectives not met may result in redoing the project or failing.</t>
-  </si>
-  <si>
-    <t>Project completed incorrectly or project incomplete.</t>
-  </si>
-  <si>
-    <t>Build-up of work to do.
-Increase workload causing overworking.</t>
-  </si>
-  <si>
-    <t>Relationship and access between data tables incorrectly defined.</t>
-  </si>
-  <si>
-    <t>Create a plan with weekly checklists.
-Project completed on-time or earlier.</t>
   </si>
   <si>
     <t>Clarify requirements if not understood.
 Project completed to the given requirements.</t>
   </si>
   <si>
-    <t>Enhance skills through additional practice.
-Improve knowledge through further research.
-Improved skills and knowledge to be able to complete the project.</t>
-  </si>
-  <si>
-    <t>Reduce internet usage of other devices.
-Keep some mobile data as back up to use.
-If connection fails, project timeline remains unaffected.</t>
-  </si>
-  <si>
-    <t>Additional research.
-Consult to confirm understanding.
-Less chance of oversights in the database.</t>
-  </si>
-  <si>
-    <t>During the creation of the ERD.</t>
-  </si>
-  <si>
-    <t>Unknown.
-Unpredictable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primarily in the early stages but may occur at any stage throughout the project. </t>
-  </si>
-  <si>
     <t>Early stages, beginning of the project when objectives are stated.</t>
   </si>
   <si>
@@ -180,18 +127,12 @@
     <t>16.04.2020</t>
   </si>
   <si>
-    <t>Avoid</t>
-  </si>
-  <si>
     <t>Misunderstanding project scope</t>
   </si>
   <si>
     <t>Illness/Injury</t>
   </si>
   <si>
-    <t>Long term</t>
-  </si>
-  <si>
     <t>Medium term issue and instance of occurrence unpredictable.</t>
   </si>
   <si>
@@ -207,10 +148,115 @@
     <t>H</t>
   </si>
   <si>
-    <t xml:space="preserve">Git </t>
-  </si>
-  <si>
     <t>25.04.2020</t>
+  </si>
+  <si>
+    <t>29.04.2020</t>
+  </si>
+  <si>
+    <t>Short term impact. Issue would be identified when inputting data to the databases tables.</t>
+  </si>
+  <si>
+    <t>Not reading and identifying the requirements correctly.</t>
+  </si>
+  <si>
+    <t>Time allocated to each aspect of the project not clearly defined.</t>
+  </si>
+  <si>
+    <t>Overlap of individual feature timelines which creates a backlog and delay in project completion.</t>
+  </si>
+  <si>
+    <t>Create a realistic deadline for each feature to be designed.</t>
+  </si>
+  <si>
+    <t>27.04.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing failures </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Git push </t>
+  </si>
+  <si>
+    <t>Avoid or limit human contact to bare necessities.</t>
+  </si>
+  <si>
+    <t>Short term but variable depending on illness.</t>
+  </si>
+  <si>
+    <t>Long term.</t>
+  </si>
+  <si>
+    <t>Short term, initial stage of the project or for new implementations.</t>
+  </si>
+  <si>
+    <t>Research practices required for implementation of new features.</t>
+  </si>
+  <si>
+    <t>Insufficient practice on programming language and mediocre knowledge of technologies to be used.</t>
+  </si>
+  <si>
+    <t>Database and its tables created incorrectly.</t>
+  </si>
+  <si>
+    <t>Short term issue,  but unpredictable.</t>
+  </si>
+  <si>
+    <t>Developer lacks mobility and is unable to start or continue or finish the project.</t>
+  </si>
+  <si>
+    <t>Workload bulds-up and if developer does not recover before project deadline, project is incomplete.</t>
+  </si>
+  <si>
+    <t>Low quality project developed, many of the requirements are not met.</t>
+  </si>
+  <si>
+    <t>Design an ERD which immitates the databases tables correctly and test it before advancing in the project.</t>
+  </si>
+  <si>
+    <t>Unable to upload files to the git repository.</t>
+  </si>
+  <si>
+    <t>Presentation questions</t>
+  </si>
+  <si>
+    <t>Avoid: Only upload from a single device to avoid merge conflicts.</t>
+  </si>
+  <si>
+    <t>Short term.</t>
+  </si>
+  <si>
+    <t>Avoid: Reduce internet usage of other devices. Use mySQL workbench on device whenever internet is down.</t>
+  </si>
+  <si>
+    <t>Not well prepared to answer questions.</t>
+  </si>
+  <si>
+    <t>Short term, occuring at the end of the project.</t>
+  </si>
+  <si>
+    <t>Understanding of project appears to be low and unable to explain the project to a high standard.</t>
+  </si>
+  <si>
+    <t>Unable to connect to database and view information in the tables to see if JAVA code works correctly. Unable to push files to nexus.</t>
+  </si>
+  <si>
+    <t>Low coverage of testing for the code developed.</t>
+  </si>
+  <si>
+    <t>Solve: Errors in code require refactoring to be able to pass the tests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium term. </t>
+  </si>
+  <si>
+    <t>Delays in uploading working features.</t>
+  </si>
+  <si>
+    <t>Application not functioning as required so project requirements not met.</t>
+  </si>
+  <si>
+    <t>Recap everything done to date to reaffirm understanding.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -476,23 +522,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672790C0-2960-4938-80FA-B969A373BC5B}">
-  <dimension ref="A2:M18"/>
+  <dimension ref="A2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,33 +902,33 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="19"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
     </row>
     <row r="7" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -908,7 +957,7 @@
         <v>19</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="M7" s="7" t="s">
         <v>18</v>
@@ -922,23 +971,29 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="M8" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -953,31 +1008,31 @@
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="2"/>
       <c r="I9" s="5"/>
       <c r="J9" s="4" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
-        <f t="shared" ref="A10:A18" si="0">A9+1</f>
+        <f t="shared" ref="A10:A17" si="0">A9+1</f>
         <v>3</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -987,26 +1042,26 @@
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="2"/>
       <c r="I10" s="5"/>
       <c r="J10" s="4" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1021,26 +1076,26 @@
         <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="1" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1052,29 +1107,29 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="2"/>
       <c r="I12" s="5"/>
       <c r="J12" s="4" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1083,32 +1138,32 @@
         <v>6</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="2"/>
       <c r="I13" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1117,32 +1172,32 @@
         <v>7</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4"/>
       <c r="K14" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1151,75 +1206,101 @@
         <v>8</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="B16" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="2"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="J16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>